<commit_message>
Primer commit: subiendo el sistema completo
</commit_message>
<xml_diff>
--- a/sistemaback/dashboard/dashboard_landmech.xlsx
+++ b/sistemaback/dashboard/dashboard_landmech.xlsx
@@ -3505,7 +3505,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5002,6 +5002,63 @@
       <c r="M26" t="inlineStr">
         <is>
           <t>johnny</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>46</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>45836</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>zeta</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Hornos</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>2</v>
+      </c>
+      <c r="F27" t="n">
+        <v>2</v>
+      </c>
+      <c r="G27" t="n">
+        <v>4</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Activo</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Soluciones Electromecánicas</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Almacén 4</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Inventario 2</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>REGISTRAR</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>nestor</t>
         </is>
       </c>
     </row>
@@ -5102,7 +5159,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="3" t="n">
-        <v>45836.93959595001</v>
+        <v>45838.59877830116</v>
       </c>
       <c r="H2" t="b">
         <v>1</v>
@@ -5140,16 +5197,16 @@
         <v>0</v>
       </c>
       <c r="G3" s="3" t="n">
-        <v>45836.86378440374</v>
+        <v>45837.00596537504</v>
       </c>
       <c r="H3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -5178,7 +5235,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>45835.71126851214</v>
+        <v>45837.00615547206</v>
       </c>
       <c r="H4" t="b">
         <v>1</v>
@@ -5257,13 +5314,13 @@
         <v>45836.8502850816</v>
       </c>
       <c r="H6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>